<commit_message>
perf new directory structure | 优化目录结构
</commit_message>
<xml_diff>
--- a/日志.xlsx
+++ b/日志.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>名称</t>
   </si>
@@ -55,6 +55,34 @@
   </si>
   <si>
     <t>内容需要续写，未完成状态</t>
+  </si>
+  <si>
+    <t>优化目录结构-添加（自制品、选购品）分类</t>
+  </si>
+  <si>
+    <t>优化目录</t>
+  </si>
+  <si>
+    <t>(2~7)移动至（/自制品）目录</t>
+  </si>
+  <si>
+    <t>更新目录</t>
+  </si>
+  <si>
+    <r>
+      <t>选购品/</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF800080"/>
+        <rFont val="宋体"/>
+        <charset val="0"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>推荐购买-蛋挞液-挞皮</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -62,11 +90,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="yyyy/m/d;@"/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="yyyy/m/d;@"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -86,81 +114,97 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -174,16 +218,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -197,32 +241,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -237,13 +265,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -255,169 +343,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -428,6 +456,32 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -442,39 +496,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -496,10 +517,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -509,21 +528,30 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -533,152 +561,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -686,6 +714,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1036,15 +1067,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="6" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="35.1818181818182" customWidth="1"/>
+    <col min="1" max="1" width="46.3636363636364" customWidth="1"/>
     <col min="2" max="2" width="16.7272727272727" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.9090909090909" customWidth="1"/>
     <col min="4" max="4" width="38.1818181818182" customWidth="1"/>
@@ -1131,6 +1162,39 @@
       </c>
       <c r="D7" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44716</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44716</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44716</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1141,6 +1205,7 @@
     <hyperlink ref="A5" r:id="rId4" display="咖喱牛肉"/>
     <hyperlink ref="A6" r:id="rId5" display="新奥尔良-标准卡津料理配方"/>
     <hyperlink ref="A7" r:id="rId6" display="复刻-KFC新奥尔良烤翅"/>
+    <hyperlink ref="A10" r:id="rId7" display="选购品/推荐购买-蛋挞液-挞皮"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>